<commit_message>
update Mastertable and Docu
</commit_message>
<xml_diff>
--- a/master_table/Possible_Template_TF_OntoWorldMap_2023-03-28_10-52.xlsx
+++ b/master_table/Possible_Template_TF_OntoWorldMap_2023-03-28_10-52.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Ontology-Overview-of-NFDI4Cat\Master_Table\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Ontology-Overview-of-NFDI4Cat\master_table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1AC93F-F6CE-4945-BF0D-77852B9FEEC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D080433-8361-42E4-992D-BE3EB2098F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template mit Beispiel" sheetId="4" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="397">
   <si>
     <t>Ontology</t>
   </si>
@@ -931,9 +931,6 @@
   </si>
   <si>
     <t>rdfs:label, rdf datatype(definition)</t>
-  </si>
-  <si>
-    <t>Just forget this Ontology ever existed, it is that bad!</t>
   </si>
   <si>
     <t>Egon Willighagen; Cristian Munteanu; Evan Bolton; Gang Fu; Janna Hastings; Leonid Chepelev; Mark Davies; Michel Dumontier</t>
@@ -1288,6 +1285,12 @@
       </rPr>
       <t>https://www.ebi.ac.uk/chebi/downloadsForward.do</t>
     </r>
+  </si>
+  <si>
+    <t>Ontology on Physico-chemical Processes</t>
+  </si>
+  <si>
+    <t>Not really usable, not FAIR</t>
   </si>
 </sst>
 </file>
@@ -2192,7 +2195,7 @@
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
@@ -2644,7 +2647,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -2654,7 +2657,7 @@
     </row>
     <row r="9" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -2664,7 +2667,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="28.5" x14ac:dyDescent="0.25">
@@ -2679,7 +2682,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -2689,7 +2692,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -2699,7 +2702,7 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -2709,17 +2712,17 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="28.5" x14ac:dyDescent="0.25">
@@ -2734,7 +2737,7 @@
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
@@ -2744,7 +2747,7 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
@@ -2754,7 +2757,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
@@ -2764,7 +2767,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
@@ -2774,7 +2777,7 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
@@ -2784,7 +2787,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
@@ -2794,7 +2797,7 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
@@ -2804,7 +2807,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
@@ -2814,7 +2817,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="28.5" x14ac:dyDescent="0.25">
@@ -3049,7 +3052,7 @@
     </row>
     <row r="94" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="36" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
@@ -3104,7 +3107,7 @@
     </row>
     <row r="5" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3124,7 +3127,7 @@
     </row>
     <row r="9" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3134,7 +3137,7 @@
     </row>
     <row r="11" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3149,7 +3152,7 @@
     </row>
     <row r="15" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3159,7 +3162,7 @@
     </row>
     <row r="17" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3184,12 +3187,12 @@
     </row>
     <row r="22" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3204,7 +3207,7 @@
     </row>
     <row r="27" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3214,7 +3217,7 @@
     </row>
     <row r="29" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3224,7 +3227,7 @@
     </row>
     <row r="31" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3234,7 +3237,7 @@
     </row>
     <row r="33" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3254,7 +3257,7 @@
     </row>
     <row r="37" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3274,7 +3277,7 @@
     </row>
     <row r="41" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3284,7 +3287,7 @@
     </row>
     <row r="43" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3419,7 +3422,7 @@
     </row>
     <row r="71" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3519,7 +3522,7 @@
     </row>
     <row r="93" spans="1:1" ht="90" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -3553,7 +3556,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -3583,7 +3586,7 @@
     </row>
     <row r="9" spans="1:1" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="41" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -3608,7 +3611,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -3618,7 +3621,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -3638,17 +3641,17 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="28.5" x14ac:dyDescent="0.25">
@@ -3683,7 +3686,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
@@ -3693,7 +3696,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
@@ -3713,7 +3716,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
@@ -3723,7 +3726,7 @@
     </row>
     <row r="39" spans="1:1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
@@ -3733,7 +3736,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
@@ -3743,7 +3746,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="28.5" x14ac:dyDescent="0.25">
@@ -3978,7 +3981,7 @@
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="39" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
@@ -4014,7 +4017,7 @@
   <dimension ref="A1:A126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4035,7 +4038,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>395</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -4045,7 +4048,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -4118,12 +4121,12 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
@@ -4143,7 +4146,7 @@
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
@@ -4173,7 +4176,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
@@ -4183,7 +4186,7 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
@@ -4193,7 +4196,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
@@ -4213,7 +4216,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
@@ -4223,7 +4226,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4358,7 +4361,7 @@
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
@@ -4458,7 +4461,7 @@
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="39" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
@@ -4486,8 +4489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F126"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4508,7 +4511,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -4538,7 +4541,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="63" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -4548,7 +4551,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4563,7 +4566,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -4573,7 +4576,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="21" x14ac:dyDescent="0.25">
@@ -4594,17 +4597,17 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4639,7 +4642,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -4649,7 +4652,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
@@ -4659,7 +4662,7 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
@@ -4669,7 +4672,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
@@ -4689,7 +4692,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
@@ -4699,7 +4702,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4834,7 +4837,7 @@
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
@@ -4934,7 +4937,7 @@
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="39" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
@@ -4988,7 +4991,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -5043,7 +5046,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -5053,7 +5056,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -5073,12 +5076,12 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
@@ -5108,7 +5111,7 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
@@ -5118,7 +5121,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
@@ -5128,7 +5131,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
@@ -5148,7 +5151,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
@@ -5158,7 +5161,7 @@
     </row>
     <row r="39" spans="1:1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
@@ -5168,7 +5171,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
@@ -5178,7 +5181,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="28.5" x14ac:dyDescent="0.25">
@@ -5413,7 +5416,7 @@
     </row>
     <row r="93" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A93" s="39" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
@@ -6477,7 +6480,7 @@
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
@@ -6939,7 +6942,7 @@
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
@@ -7412,7 +7415,7 @@
     </row>
     <row r="22" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7766,8 +7769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:A94"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7880,7 +7883,7 @@
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
@@ -8227,7 +8230,7 @@
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="22" t="s">
-        <v>285</v>
+        <v>396</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
@@ -8298,7 +8301,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -8333,7 +8336,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -8358,12 +8361,12 @@
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="28.5" x14ac:dyDescent="0.25">
@@ -8378,7 +8381,7 @@
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
@@ -8398,7 +8401,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
@@ -8408,7 +8411,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
@@ -8428,7 +8431,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
@@ -8438,7 +8441,7 @@
     </row>
     <row r="39" spans="1:1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
@@ -8448,7 +8451,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
@@ -8458,7 +8461,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="28.5" x14ac:dyDescent="0.25">
@@ -8693,7 +8696,7 @@
     </row>
     <row r="93" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A93" s="39" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
@@ -8749,7 +8752,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -8774,7 +8777,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -8784,7 +8787,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="28.5" x14ac:dyDescent="0.25">
@@ -8809,7 +8812,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -8834,7 +8837,7 @@
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
@@ -8852,7 +8855,7 @@
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
@@ -8872,7 +8875,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
@@ -8882,7 +8885,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
@@ -8892,7 +8895,7 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
@@ -8902,7 +8905,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
@@ -8912,7 +8915,7 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
@@ -8922,7 +8925,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
@@ -8932,7 +8935,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="28.5" x14ac:dyDescent="0.25">
@@ -9167,7 +9170,7 @@
     </row>
     <row r="94" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="36" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
@@ -9188,7 +9191,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:A95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -9220,7 +9223,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -9230,7 +9233,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -9240,7 +9243,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -9250,7 +9253,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -9265,7 +9268,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -9275,7 +9278,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -9285,7 +9288,7 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="60" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -9295,17 +9298,17 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="41" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -9320,7 +9323,7 @@
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
@@ -9340,7 +9343,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
@@ -9350,7 +9353,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
@@ -9360,7 +9363,7 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
@@ -9370,7 +9373,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
@@ -9380,7 +9383,7 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
@@ -9390,7 +9393,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
@@ -9400,7 +9403,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -9635,7 +9638,7 @@
     </row>
     <row r="94" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="36" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
@@ -9660,6 +9663,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="文档" ma:contentTypeID="0x010100E35C4A3F015220429587A6885988F55A" ma:contentTypeVersion="2" ma:contentTypeDescription="新建文档。" ma:contentTypeScope="" ma:versionID="d6504310574d90ff3af330d88d4b27c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="43c33c4e-3078-430a-a993-ec9e07a267b1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7023e3b9e2c813b12cebe0f0ea1d5cce" ns2:_="">
     <xsd:import namespace="43c33c4e-3078-430a-a993-ec9e07a267b1"/>
@@ -9791,12 +9800,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4E38D5B-D85B-4D43-8837-BDE8BD7F5B8A}">
   <ds:schemaRefs>
@@ -9806,6 +9809,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0CE3216-5465-401D-96FE-F0724F372422}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3709C412-EE61-448D-9135-2444D463CA94}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9821,13 +9833,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0CE3216-5465-401D-96FE-F0724F372422}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update Entry of OntoCAPE
</commit_message>
<xml_diff>
--- a/master_table/Possible_Template_TF_OntoWorldMap_2023-03-28_10-52.xlsx
+++ b/master_table/Possible_Template_TF_OntoWorldMap_2023-03-28_10-52.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Ontology-Overview-of-NFDI4Cat\master_table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D080433-8361-42E4-992D-BE3EB2098F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6544FE88-6BC8-497D-9016-6FF06C2B9759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template mit Beispiel" sheetId="4" r:id="rId1"/>
@@ -1092,9 +1092,6 @@
     <t>While it  sounds like the Ontology should describe Environemnts and its relations, such as 'Lake' 'canBePoisonedBy' 'CopperSalt' or 'Windturbine' 'generates('NoisePolution' 'some' 'dB')', it is more of a "biome-ontology", descriptions of local/abstract environments end a e.g. Wastefills.</t>
   </si>
   <si>
-    <t>ontology for the domain of Computer Aided Process Engineering</t>
-  </si>
-  <si>
     <t>RWTH Aachen University</t>
   </si>
   <si>
@@ -1291,6 +1288,9 @@
   </si>
   <si>
     <t>Not really usable, not FAIR</t>
+  </si>
+  <si>
+    <t>Ontology for the domain of Computer Aided Process Engineering</t>
   </si>
 </sst>
 </file>
@@ -2195,7 +2195,7 @@
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
@@ -2717,7 +2717,7 @@
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
@@ -3075,8 +3075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:A93"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3097,7 +3097,7 @@
     </row>
     <row r="3" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>396</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3107,7 +3107,7 @@
     </row>
     <row r="5" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>338</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3127,7 +3127,7 @@
     </row>
     <row r="9" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3137,7 +3137,7 @@
     </row>
     <row r="11" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3152,7 +3152,7 @@
     </row>
     <row r="15" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3162,7 +3162,7 @@
     </row>
     <row r="17" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3187,12 +3187,12 @@
     </row>
     <row r="22" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3217,7 +3217,7 @@
     </row>
     <row r="29" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3227,7 +3227,7 @@
     </row>
     <row r="31" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3237,7 +3237,7 @@
     </row>
     <row r="33" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3257,7 +3257,7 @@
     </row>
     <row r="37" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3277,7 +3277,7 @@
     </row>
     <row r="41" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3287,7 +3287,7 @@
     </row>
     <row r="43" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3422,7 +3422,7 @@
     </row>
     <row r="71" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3522,7 +3522,7 @@
     </row>
     <row r="93" spans="1:1" ht="90" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -3556,7 +3556,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -3586,7 +3586,7 @@
     </row>
     <row r="9" spans="1:1" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="41" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -3611,7 +3611,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -3621,7 +3621,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -3641,17 +3641,17 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="28.5" x14ac:dyDescent="0.25">
@@ -3686,7 +3686,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
@@ -3696,7 +3696,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
@@ -3716,7 +3716,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
@@ -3736,7 +3736,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
@@ -3746,7 +3746,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="28.5" x14ac:dyDescent="0.25">
@@ -3981,7 +3981,7 @@
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="39" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
@@ -4038,7 +4038,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -4048,7 +4048,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -4121,12 +4121,12 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
@@ -4176,7 +4176,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
@@ -4186,7 +4186,7 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
@@ -4196,7 +4196,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
@@ -4216,7 +4216,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
@@ -4226,7 +4226,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4361,7 +4361,7 @@
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
@@ -4461,7 +4461,7 @@
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="39" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
@@ -4541,7 +4541,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="63" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -4551,7 +4551,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4566,7 +4566,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -4576,7 +4576,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="21" x14ac:dyDescent="0.25">
@@ -4597,17 +4597,17 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4642,7 +4642,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -4652,7 +4652,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
@@ -4662,7 +4662,7 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
@@ -4692,7 +4692,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
@@ -4702,7 +4702,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4937,7 +4937,7 @@
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="39" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
@@ -4991,7 +4991,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -5046,7 +5046,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -5056,7 +5056,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="21" x14ac:dyDescent="0.25">
@@ -5076,12 +5076,12 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
@@ -5111,7 +5111,7 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
@@ -5121,7 +5121,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
@@ -5131,7 +5131,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
@@ -5151,7 +5151,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
@@ -5161,7 +5161,7 @@
     </row>
     <row r="39" spans="1:1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
@@ -5171,7 +5171,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
@@ -5181,7 +5181,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="28.5" x14ac:dyDescent="0.25">
@@ -5416,7 +5416,7 @@
     </row>
     <row r="93" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A93" s="39" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
@@ -6480,7 +6480,7 @@
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
@@ -6942,7 +6942,7 @@
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
@@ -7415,7 +7415,7 @@
     </row>
     <row r="22" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7769,7 +7769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:A94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+    <sheetView topLeftCell="A72" workbookViewId="0">
       <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
@@ -7883,7 +7883,7 @@
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
@@ -8230,7 +8230,7 @@
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="22" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
@@ -8361,7 +8361,7 @@
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
@@ -8837,7 +8837,7 @@
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
@@ -9303,12 +9303,12 @@
     </row>
     <row r="22" spans="1:1" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="41" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -9663,12 +9663,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="文档" ma:contentTypeID="0x010100E35C4A3F015220429587A6885988F55A" ma:contentTypeVersion="2" ma:contentTypeDescription="新建文档。" ma:contentTypeScope="" ma:versionID="d6504310574d90ff3af330d88d4b27c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="43c33c4e-3078-430a-a993-ec9e07a267b1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7023e3b9e2c813b12cebe0f0ea1d5cce" ns2:_="">
     <xsd:import namespace="43c33c4e-3078-430a-a993-ec9e07a267b1"/>
@@ -9800,6 +9794,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4E38D5B-D85B-4D43-8837-BDE8BD7F5B8A}">
   <ds:schemaRefs>
@@ -9809,15 +9809,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0CE3216-5465-401D-96FE-F0724F372422}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3709C412-EE61-448D-9135-2444D463CA94}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9833,4 +9824,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0CE3216-5465-401D-96FE-F0724F372422}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>